<commit_message>
+ hiv ba results
</commit_message>
<xml_diff>
--- a/dependent_mediators/results_real_data2.xlsx
+++ b/dependent_mediators/results_real_data2.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="rf+or" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="linear+or" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,228 +426,228 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>heart disorder</t>
+          <t>abuse</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24.731 [27.355 -- 27.355]</t>
+          <t>69.668 [36.641 -- 89.251]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>75.269 [72.645 -- 72.645]</t>
+          <t>30.332 [10.749 -- 63.359]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.034 [0.060 -- 0.060]</t>
+          <t>0.810 [0.243 -- 2.105]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.103 [0.159 -- 0.159]</t>
+          <t>0.353 [0.141 -- 0.750]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.137 [0.219 -- 0.219]</t>
+          <t>1.163 [0.584 -- 2.630]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.952 [1.246 -- 1.246]</t>
+          <t>1.315 [0.657 -- 2.159]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.948 [1.247 -- 1.247]</t>
+          <t>1.297 [0.625 -- 2.103]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.754 [0.817 -- 0.817]</t>
+          <t>0.647 [0.596 -- 0.754]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.776 [0.783 -- 0.783]</t>
+          <t>0.639 [0.628 -- 0.672]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>-10.084 [-10.092 -- -10.092]</t>
+          <t>-10.067 [-10.346 -- -9.734]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>avg</t>
+          <t>heart disorder</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>69.237 [66.418 -- 66.418]</t>
+          <t>77.584 [52.898 -- 94.606]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30.763 [33.582 -- 33.582]</t>
+          <t>22.416 [5.394 -- 47.102]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.095 [0.145 -- 0.145]</t>
+          <t>0.903 [0.342 -- 2.384]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.042 [0.073 -- 0.073]</t>
+          <t>0.261 [0.067 -- 0.526]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.137 [0.219 -- 0.219]</t>
+          <t>1.164 [0.585 -- 2.632]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.767 [0.689 -- 0.689]</t>
+          <t>1.129 [0.547 -- 1.965]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.746 [0.674 -- 0.674]</t>
+          <t>1.126 [0.520 -- 1.950]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.754 [0.817 -- 0.817]</t>
+          <t>0.647 [0.596 -- 0.754]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>nan [nan -- nan]</t>
+          <t>0.786 [0.771 -- 0.803]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-10.084 [-10.092 -- -10.092]</t>
+          <t>-10.067 [-10.346 -- -9.734]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sleep disorder</t>
+          <t>avg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>89.399 [99.225 -- 99.225]</t>
+          <t>80.314 [61.774 -- 89.459]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10.601 [0.775 -- 0.775]</t>
+          <t>19.686 [10.541 -- 38.226]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.122 [0.217 -- 0.217]</t>
+          <t>0.935 [0.391 -- 2.293]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.015 [0.002 -- 0.002]</t>
+          <t>0.229 [0.127 -- 0.424]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.137 [0.219 -- 0.219]</t>
+          <t>1.164 [0.585 -- 2.631]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.145 [0.026 -- 0.026]</t>
+          <t>0.959 [0.578 -- 1.430]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.147 [0.030 -- 0.030]</t>
+          <t>0.952 [0.573 -- 1.396]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.754 [0.817 -- 0.817]</t>
+          <t>0.647 [0.596 -- 0.754]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.648 [0.639 -- 0.639]</t>
+          <t>nan [nan -- nan]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>-10.084 [-10.092 -- -10.092]</t>
+          <t>-10.067 [-10.346 -- -9.734]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>abuse</t>
+          <t>sleep disorder</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>93.357 [72.667 -- 72.667]</t>
+          <t>93.686 [71.436 -- 103.977]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.643 [27.333 -- 27.333]</t>
+          <t>6.314 [-3.977 -- 28.564]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.129 [0.159 -- 0.159]</t>
+          <t>1.090 [0.480 -- 2.426]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.009 [0.060 -- 0.060]</t>
+          <t>0.073 [-0.048 -- 0.371]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.138 [0.219 -- 0.219]</t>
+          <t>1.164 [0.585 -- 2.632]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1.206 [0.794 -- 0.794]</t>
+          <t>0.433 [-0.145 -- 1.090]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1.142 [0.744 -- 0.744]</t>
+          <t>0.433 [-0.145 -- 1.090]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.754 [0.817 -- 0.817]</t>
+          <t>0.647 [0.596 -- 0.754]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.640 [0.648 -- 0.648]</t>
+          <t>0.641 [0.626 -- 0.666]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>-10.084 [-10.092 -- -10.092]</t>
+          <t>-10.067 [-10.346 -- -9.734]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
+ hiv brain age code
</commit_message>
<xml_diff>
--- a/dependent_mediators/results_real_data2.xlsx
+++ b/dependent_mediators/results_real_data2.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="linear+or" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="linear+dr" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,228 +426,228 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>abuse</t>
+          <t>obesity</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>69.668 [36.641 -- 89.251]</t>
+          <t>22.457 [57.334 -- 57.334]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30.332 [10.749 -- 63.359]</t>
+          <t>77.543 [42.666 -- 42.666]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.810 [0.243 -- 2.105]</t>
+          <t>2.644 [7.652 -- 7.652]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.353 [0.141 -- 0.750]</t>
+          <t>9.131 [5.694 -- 5.694]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.163 [0.584 -- 2.630]</t>
+          <t>11.775 [13.346 -- 13.346]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.315 [0.657 -- 2.159]</t>
+          <t>-0.323 [-0.627 -- -0.627]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.297 [0.625 -- 2.103]</t>
+          <t>8.156 [1.377 -- 1.377]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.647 [0.596 -- 0.754]</t>
+          <t>0.727 [0.754 -- 0.754]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.639 [0.628 -- 0.672]</t>
+          <t>0.778 [0.781 -- 0.781]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>-10.067 [-10.346 -- -9.734]</t>
+          <t>-10.066 [-10.024 -- -10.024]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>heart disorder</t>
+          <t>avg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>77.584 [52.898 -- 94.606]</t>
+          <t>46.566 [51.378 -- 51.378]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22.416 [5.394 -- 47.102]</t>
+          <t>53.434 [48.622 -- 48.622]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.903 [0.342 -- 2.384]</t>
+          <t>4.324 [6.228 -- 6.228]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.261 [0.067 -- 0.526]</t>
+          <t>4.962 [5.893 -- 5.893]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.164 [0.585 -- 2.632]</t>
+          <t>9.286 [12.121 -- 12.121]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1.129 [0.547 -- 1.965]</t>
+          <t>0.256 [-0.164 -- -0.164]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1.126 [0.520 -- 1.950]</t>
+          <t>4.275 [1.840 -- 1.840]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.647 [0.596 -- 0.754]</t>
+          <t>0.727 [0.754 -- 0.754]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.786 [0.771 -- 0.803]</t>
+          <t>nan [nan -- nan]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-10.067 [-10.346 -- -9.734]</t>
+          <t>-10.066 [-10.024 -- -10.024]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>avg</t>
+          <t>sleep disorder</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>80.314 [61.774 -- 89.459]</t>
+          <t>57.381 [93.875 -- 93.875]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>19.686 [10.541 -- 38.226]</t>
+          <t>42.619 [6.125 -- 6.125]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.935 [0.391 -- 2.293]</t>
+          <t>5.328 [11.537 -- 11.537]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.229 [0.127 -- 0.424]</t>
+          <t>3.958 [0.753 -- 0.753]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1.164 [0.585 -- 2.631]</t>
+          <t>9.286 [12.289 -- 12.289]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.959 [0.578 -- 1.430]</t>
+          <t>0.404 [0.539 -- 0.539]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.952 [0.573 -- 1.396]</t>
+          <t>2.212 [-7.821 -- -7.821]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.647 [0.596 -- 0.754]</t>
+          <t>0.727 [0.754 -- 0.754]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>nan [nan -- nan]</t>
+          <t>0.617 [0.623 -- 0.623]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>-10.067 [-10.346 -- -9.734]</t>
+          <t>-10.066 [-10.024 -- -10.024]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sleep disorder</t>
+          <t>heart disorder</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>93.686 [71.436 -- 103.977]</t>
+          <t>73.558 [-4.715 -- -4.715]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.314 [-3.977 -- 28.564]</t>
+          <t>26.442 [104.715 -- 104.715]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.090 [0.480 -- 2.426]</t>
+          <t>5.000 [-0.506 -- -0.506]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.073 [-0.048 -- 0.371]</t>
+          <t>1.797 [11.233 -- 11.233]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1.164 [0.585 -- 2.632]</t>
+          <t>6.797 [10.728 -- 10.728]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.433 [-0.145 -- 1.090]</t>
+          <t>0.687 [-0.405 -- -0.405]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.433 [-0.145 -- 1.090]</t>
+          <t>2.457 [11.964 -- 11.964]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.647 [0.596 -- 0.754]</t>
+          <t>0.727 [0.754 -- 0.754]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.641 [0.626 -- 0.666]</t>
+          <t>0.735 [0.740 -- 0.740]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>-10.067 [-10.346 -- -9.734]</t>
+          <t>-10.066 [-10.024 -- -10.024]</t>
         </is>
       </c>
     </row>

</xml_diff>